<commit_message>
Third commit Uploaded: source code draft -solved errors(login form), additional classes
</commit_message>
<xml_diff>
--- a/Proiect colectiv - planificare task-uri.xlsx
+++ b/Proiect colectiv - planificare task-uri.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PC - Administrare universitate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planificare pe săptămâni" sheetId="1" r:id="rId1"/>
+    <sheet name="Operații posibile pt useri" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
   <si>
     <t>Andreea</t>
   </si>
@@ -83,28 +84,121 @@
     <t>realizare fereastră de login</t>
   </si>
   <si>
-    <t>realizare fereastră de vizualizare studenți, facultăți, profesori(tabel)</t>
-  </si>
-  <si>
-    <t>&lt;-- continuare</t>
-  </si>
-  <si>
     <t>debugging</t>
   </si>
   <si>
-    <t>îmbunătățire interfață grafică utilizând PS</t>
-  </si>
-  <si>
-    <t>realizare fereastră de managing(studenți, cursuri, profesori etc.)</t>
-  </si>
-  <si>
     <t>creare clase inițiale necesare(User, Manager GUI etc.)</t>
   </si>
   <si>
-    <t>realizare fereastră de meniu(corespunzătoare fiecărui tip de user)</t>
-  </si>
-  <si>
     <t>creare și populare tabele pentru DB(2)</t>
+  </si>
+  <si>
+    <t>documentare pentru realizarea de elemente grafice(butoane, iconițe etc)</t>
+  </si>
+  <si>
+    <t>Perspective/Ferestre de operații</t>
+  </si>
+  <si>
+    <t>Secretariat</t>
+  </si>
+  <si>
+    <t>Administrație/rectorat</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Profesor</t>
+  </si>
+  <si>
+    <t>Adăugare/eliminare/modificare facultăți/specializări</t>
+  </si>
+  <si>
+    <t>Adăugare/eliminare/modificare studenți</t>
+  </si>
+  <si>
+    <t>Adăugare/eliminare/modificare profesori</t>
+  </si>
+  <si>
+    <t>Vizualizare note</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Vizualizare informații profesori</t>
+  </si>
+  <si>
+    <t>Vizualizare informații studenți</t>
+  </si>
+  <si>
+    <t>Formular de contact</t>
+  </si>
+  <si>
+    <t>realizare meniu pt admin</t>
+  </si>
+  <si>
+    <t>realizare elemente grafice(butoane, iconițe etc.)</t>
+  </si>
+  <si>
+    <t>&lt;--continuare</t>
+  </si>
+  <si>
+    <t>realizare formular de contact</t>
+  </si>
+  <si>
+    <t>realizare mini-ghid de help/utilizare</t>
+  </si>
+  <si>
+    <t>Adăugare note</t>
+  </si>
+  <si>
+    <t>Eliminare/modificare note</t>
+  </si>
+  <si>
+    <t>Adăugare/eliminare/modificare materii</t>
+  </si>
+  <si>
+    <t>Număr de ferestre</t>
+  </si>
+  <si>
+    <t>3(toate notele pt admin+secretariat, notele la materiile predate pt profesor, note proprii pt student)</t>
+  </si>
+  <si>
+    <t>2(toți profesorii pt admin+secretariat, info personale pt profesor)</t>
+  </si>
+  <si>
+    <t>2(toți studenții pt admin+secretariat, info personale pt student)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>realizare fereastre de meniu pt fiecare tip de user</t>
+  </si>
+  <si>
+    <t>realizare meniu pt secretariat</t>
+  </si>
+  <si>
+    <t>realizare documentație</t>
+  </si>
+  <si>
+    <t>Vizualizare informații facultăți + specializări + materii</t>
+  </si>
+  <si>
+    <t>realizare fereastră de vizualizare facultăți, specializări și materii</t>
+  </si>
+  <si>
+    <t>realizare ferestre pentru vizualizare profesori, studenți(pt admin)</t>
+  </si>
+  <si>
+    <t>realizare meniu pt profesor</t>
+  </si>
+  <si>
+    <t>realizare meniu pt student</t>
   </si>
 </sst>
 </file>
@@ -275,7 +369,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -294,13 +388,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -314,15 +402,38 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -338,7 +449,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -622,84 +732,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="65" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.77734375" style="6"/>
     <col min="2" max="2" width="40.77734375" style="7"/>
-    <col min="3" max="3" width="40.77734375" style="9"/>
+    <col min="3" max="3" width="40.77734375" style="8"/>
     <col min="4" max="4" width="40.77734375" style="7"/>
-    <col min="5" max="5" width="40.77734375" style="9"/>
+    <col min="5" max="5" width="40.77734375" style="8"/>
     <col min="6" max="6" width="40.77734375" style="7"/>
-    <col min="7" max="7" width="40.77734375" style="9"/>
+    <col min="7" max="7" width="40.77734375" style="8"/>
     <col min="8" max="8" width="40.77734375" style="7"/>
-    <col min="9" max="9" width="40.77734375" style="9"/>
+    <col min="9" max="9" width="40.77734375" style="8"/>
     <col min="10" max="10" width="40.77734375" style="7"/>
-    <col min="11" max="11" width="40.77734375" style="9"/>
+    <col min="11" max="11" width="40.77734375" style="8"/>
     <col min="12" max="12" width="40.77734375" style="7"/>
-    <col min="13" max="13" width="40.77734375" style="9"/>
+    <col min="13" max="13" width="40.77734375" style="8"/>
     <col min="14" max="14" width="40.77734375" style="7"/>
-    <col min="15" max="15" width="40.77734375" style="9"/>
+    <col min="15" max="15" width="40.77734375" style="8"/>
     <col min="16" max="16" width="40.77734375" style="7"/>
-    <col min="17" max="17" width="40.77734375" style="9"/>
+    <col min="17" max="17" width="40.77734375" style="8"/>
     <col min="18" max="18" width="40.77734375" style="7"/>
-    <col min="19" max="19" width="40.77734375" style="9"/>
+    <col min="19" max="19" width="40.77734375" style="8"/>
     <col min="20" max="20" width="40.77734375" style="7"/>
-    <col min="21" max="21" width="40.77734375" style="9"/>
+    <col min="21" max="21" width="40.77734375" style="8"/>
     <col min="22" max="22" width="40.77734375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="4" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19" t="s">
+      <c r="F1" s="26"/>
+      <c r="G1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19" t="s">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19" t="s">
+      <c r="J1" s="26"/>
+      <c r="K1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19" t="s">
+      <c r="N1" s="26"/>
+      <c r="O1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19" t="s">
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19" t="s">
+      <c r="R1" s="26"/>
+      <c r="S1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19" t="s">
+      <c r="T1" s="26"/>
+      <c r="U1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="19"/>
-      <c r="W1" s="11"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" s="3" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -770,77 +880,106 @@
       </c>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="14" t="s">
+      <c r="F3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="14" t="s">
+      <c r="I3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="25"/>
+      <c r="S3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="U3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="17"/>
-      <c r="S3" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="T3" s="17"/>
-      <c r="U3" s="16" t="s">
+      <c r="V3" s="24"/>
+    </row>
+    <row r="4" spans="1:23" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="G4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="V3" s="18"/>
-    </row>
-    <row r="4" spans="1:23" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="G4" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="15"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="14"/>
+      <c r="L4" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="14"/>
+      <c r="S4" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+    </row>
+    <row r="5" spans="1:23" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="14"/>
+      <c r="O5" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="S4:V4"/>
     <mergeCell ref="U3:V3"/>
     <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
@@ -852,4 +991,274 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.77734375" customWidth="1"/>
+    <col min="2" max="5" width="10.77734375" style="17" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" style="18"/>
+    <col min="7" max="7" width="45.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="18">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fifth commit Uploaded: Menu GUI for each user
</commit_message>
<xml_diff>
--- a/Proiect colectiv - planificare task-uri.xlsx
+++ b/Proiect colectiv - planificare task-uri.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="61">
   <si>
     <t>Andreea</t>
   </si>
@@ -87,9 +87,6 @@
     <t>debugging</t>
   </si>
   <si>
-    <t>creare clase inițiale necesare(User, Manager GUI etc.)</t>
-  </si>
-  <si>
     <t>creare și populare tabele pentru DB(2)</t>
   </si>
   <si>
@@ -138,18 +135,9 @@
     <t>Formular de contact</t>
   </si>
   <si>
-    <t>realizare meniu pt admin</t>
-  </si>
-  <si>
     <t>realizare elemente grafice(butoane, iconițe etc.)</t>
   </si>
   <si>
-    <t>&lt;--continuare</t>
-  </si>
-  <si>
-    <t>realizare formular de contact</t>
-  </si>
-  <si>
     <t>realizare mini-ghid de help/utilizare</t>
   </si>
   <si>
@@ -180,32 +168,53 @@
     <t>realizare fereastre de meniu pt fiecare tip de user</t>
   </si>
   <si>
-    <t>realizare meniu pt secretariat</t>
-  </si>
-  <si>
     <t>realizare documentație</t>
   </si>
   <si>
     <t>Vizualizare informații facultăți + specializări + materii</t>
   </si>
   <si>
-    <t>realizare fereastră de vizualizare facultăți, specializări și materii</t>
-  </si>
-  <si>
-    <t>realizare ferestre pentru vizualizare profesori, studenți(pt admin)</t>
-  </si>
-  <si>
-    <t>realizare meniu pt profesor</t>
-  </si>
-  <si>
-    <t>realizare meniu pt student</t>
+    <t>creare clase inițiale necesare(Student, Profesor, Manager GUI etc.)</t>
+  </si>
+  <si>
+    <t>realizare fereastre pt vizualizare facultăți, specializări și materii</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>realizare ferestre pt vizualizare note(profesor, student)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> continuare sapt precedenta</t>
+  </si>
+  <si>
+    <t>realizare ferestre pt vizualizare profesori, studenți(admin+secretariat)</t>
+  </si>
+  <si>
+    <t>realizare fereastra pt vizualizare note(admin+secretariat)</t>
+  </si>
+  <si>
+    <t>realizare fereastra editare note(admin + secretariat)</t>
+  </si>
+  <si>
+    <t>realizare fereastra editare studenti(admin + secretariat)</t>
+  </si>
+  <si>
+    <t>realizare ferestre editare facultati, profesori(admin)</t>
+  </si>
+  <si>
+    <t>realizare fereastra vizualizare date personale(student, profesor)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> realizare fereastra editare note(profesor)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,8 +236,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +268,11 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -363,13 +384,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -380,23 +402,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -422,6 +435,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -431,29 +460,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -734,243 +764,250 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.77734375" style="6"/>
-    <col min="2" max="2" width="40.77734375" style="7"/>
-    <col min="3" max="3" width="40.77734375" style="8"/>
-    <col min="4" max="4" width="40.77734375" style="7"/>
-    <col min="5" max="5" width="40.77734375" style="8"/>
-    <col min="6" max="6" width="40.77734375" style="7"/>
-    <col min="7" max="7" width="40.77734375" style="8"/>
-    <col min="8" max="8" width="40.77734375" style="7"/>
-    <col min="9" max="9" width="40.77734375" style="8"/>
-    <col min="10" max="10" width="40.77734375" style="7"/>
-    <col min="11" max="11" width="40.77734375" style="8"/>
-    <col min="12" max="12" width="40.77734375" style="7"/>
-    <col min="13" max="13" width="40.77734375" style="8"/>
-    <col min="14" max="14" width="40.77734375" style="7"/>
-    <col min="15" max="15" width="40.77734375" style="8"/>
-    <col min="16" max="16" width="40.77734375" style="7"/>
-    <col min="17" max="17" width="40.77734375" style="8"/>
-    <col min="18" max="18" width="40.77734375" style="7"/>
-    <col min="19" max="19" width="40.77734375" style="8"/>
-    <col min="20" max="20" width="40.77734375" style="7"/>
-    <col min="21" max="21" width="40.77734375" style="8"/>
-    <col min="22" max="22" width="40.77734375" style="7"/>
+    <col min="1" max="1" width="40.77734375" style="5"/>
+    <col min="2" max="2" width="40.77734375" style="6"/>
+    <col min="3" max="3" width="40.77734375" style="7"/>
+    <col min="4" max="4" width="40.77734375" style="6"/>
+    <col min="5" max="5" width="40.77734375" style="7"/>
+    <col min="6" max="6" width="40.77734375" style="6"/>
+    <col min="7" max="7" width="40.77734375" style="7"/>
+    <col min="8" max="8" width="40.77734375" style="6"/>
+    <col min="9" max="9" width="40.77734375" style="7"/>
+    <col min="10" max="10" width="40.77734375" style="6"/>
+    <col min="11" max="11" width="40.77734375" style="7"/>
+    <col min="12" max="12" width="40.77734375" style="6"/>
+    <col min="13" max="13" width="40.77734375" style="7"/>
+    <col min="14" max="14" width="40.77734375" style="6"/>
+    <col min="15" max="15" width="40.77734375" style="7"/>
+    <col min="16" max="16" width="40.77734375" style="6"/>
+    <col min="17" max="17" width="40.77734375" style="7"/>
+    <col min="18" max="18" width="40.77734375" style="6"/>
+    <col min="19" max="19" width="40.77734375" style="7"/>
+    <col min="20" max="20" width="40.77734375" style="6"/>
+    <col min="21" max="21" width="40.77734375" style="7"/>
+    <col min="22" max="22" width="40.77734375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:23" s="20" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26" t="s">
+      <c r="F1" s="28"/>
+      <c r="G1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26" t="s">
+      <c r="H1" s="28"/>
+      <c r="I1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26" t="s">
+      <c r="L1" s="28"/>
+      <c r="M1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26" t="s">
+      <c r="N1" s="28"/>
+      <c r="O1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26" t="s">
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26" t="s">
+      <c r="R1" s="28"/>
+      <c r="S1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26" t="s">
+      <c r="T1" s="28"/>
+      <c r="U1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="26"/>
-      <c r="W1" s="9"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="19"/>
     </row>
     <row r="2" spans="1:23" s="3" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="R3" s="25"/>
+      <c r="S3" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="29"/>
+      <c r="U3" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3" s="27"/>
+    </row>
+    <row r="4" spans="1:23" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="G4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="H4" s="10"/>
+      <c r="J4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="R3" s="25"/>
-      <c r="S3" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="T3" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="U3" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="V3" s="24"/>
-    </row>
-    <row r="4" spans="1:23" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="28"/>
-      <c r="G4" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14" t="s">
+      <c r="M4" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="O4" s="14"/>
-      <c r="S4" s="22" t="s">
+      <c r="N4" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
+      <c r="O4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
     </row>
     <row r="5" spans="1:23" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I5" s="14"/>
-      <c r="O5" s="14"/>
+      <c r="O5" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C1:D1"/>
@@ -987,6 +1024,7 @@
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="S3:T3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1004,256 +1042,256 @@
   <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.77734375" customWidth="1"/>
-    <col min="2" max="5" width="10.77734375" style="17" customWidth="1"/>
-    <col min="6" max="6" width="30.77734375" style="18"/>
+    <col min="2" max="5" width="10.77734375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" style="15"/>
     <col min="7" max="7" width="45.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="D1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>45</v>
+      <c r="F1" s="17" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="18">
+        <v>27</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="15">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="18">
+        <v>28</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="18">
+        <v>29</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="18">
+        <v>38</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="18">
+        <v>39</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="18">
+        <v>40</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>46</v>
+        <v>30</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="18">
+        <v>48</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>47</v>
+      <c r="B10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>48</v>
+        <v>34</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="18">
+        <v>35</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="18">
+        <v>45</v>
+      </c>
+      <c r="F13" s="15">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sixth commit Uploaded: login form connection solved
</commit_message>
<xml_diff>
--- a/Proiect colectiv - planificare task-uri.xlsx
+++ b/Proiect colectiv - planificare task-uri.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
   <si>
     <t>Andreea</t>
   </si>
@@ -138,9 +138,6 @@
     <t>realizare elemente grafice(butoane, iconițe etc.)</t>
   </si>
   <si>
-    <t>realizare mini-ghid de help/utilizare</t>
-  </si>
-  <si>
     <t>Adăugare note</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>realizare fereastre de meniu pt fiecare tip de user</t>
-  </si>
-  <si>
     <t>realizare documentație</t>
   </si>
   <si>
@@ -177,37 +171,43 @@
     <t>creare clase inițiale necesare(Student, Profesor, Manager GUI etc.)</t>
   </si>
   <si>
-    <t>realizare fereastre pt vizualizare facultăți, specializări și materii</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>realizare ferestre pt vizualizare note(profesor, student)</t>
   </si>
   <si>
-    <t xml:space="preserve"> continuare sapt precedenta</t>
-  </si>
-  <si>
     <t>realizare ferestre pt vizualizare profesori, studenți(admin+secretariat)</t>
   </si>
   <si>
-    <t>realizare fereastra pt vizualizare note(admin+secretariat)</t>
-  </si>
-  <si>
-    <t>realizare fereastra editare note(admin + secretariat)</t>
-  </si>
-  <si>
-    <t>realizare fereastra editare studenti(admin + secretariat)</t>
-  </si>
-  <si>
-    <t>realizare ferestre editare facultati, profesori(admin)</t>
-  </si>
-  <si>
-    <t>realizare fereastra vizualizare date personale(student, profesor)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> realizare fereastra editare note(profesor)</t>
+    <t>realizare ferestre pt vizualizare facultăți, specializări și materii</t>
+  </si>
+  <si>
+    <t>realizare ferestre de meniu pt fiecare tip de user</t>
+  </si>
+  <si>
+    <t>realizare fereastră vizualizare date personale(student, profesor)</t>
+  </si>
+  <si>
+    <t>realizare fereastră editare note(admin + secretariat)</t>
+  </si>
+  <si>
+    <t>realizare fereastră editare studenti(admin + secretariat)</t>
+  </si>
+  <si>
+    <t>realizare ferestre editare facultăți, profesori(admin)</t>
+  </si>
+  <si>
+    <t>realizare fereastră editare note(profesor)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> continuare săpt precedentă</t>
+  </si>
+  <si>
+    <t>adăugare funcționalitate ferestre</t>
+  </si>
+  <si>
+    <t>realizare ferestre pt vizualizare note(admin+secretariat)</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -476,6 +476,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -764,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -924,44 +930,46 @@
         <v>17</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>59</v>
+      <c r="I3" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L3" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="R3" s="25"/>
+      <c r="Q3" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" s="35" t="s">
+        <v>58</v>
+      </c>
       <c r="S3" s="26" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="T3" s="29"/>
       <c r="U3" s="26" t="s">
@@ -979,25 +987,25 @@
       </c>
       <c r="H4" s="10"/>
       <c r="J4" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>60</v>
-      </c>
       <c r="S4" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="T4" s="25"/>
       <c r="U4" s="25"/>
@@ -1007,7 +1015,7 @@
       <c r="O5" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C1:D1"/>
@@ -1016,7 +1024,6 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="S4:V4"/>
     <mergeCell ref="U3:V3"/>
-    <mergeCell ref="Q3:R3"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
@@ -1064,7 +1071,7 @@
         <v>25</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1129,7 +1136,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>31</v>
@@ -1149,7 +1156,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>31</v>
@@ -1169,7 +1176,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>31</v>
@@ -1204,12 +1211,12 @@
         <v>31</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>31</v>
@@ -1244,7 +1251,7 @@
         <v>32</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1264,7 +1271,7 @@
         <v>31</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1289,7 +1296,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" s="15">
         <v>27</v>

</xml_diff>